<commit_message>
13/12/2023 give advices by fc
</commit_message>
<xml_diff>
--- a/sinh/suy diễn.xlsx
+++ b/sinh/suy diễn.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ptiteduvn-my.sharepoint.com/personal/huytq_b20cn327_stu_ptit_edu_vn/Documents/Desktop/CHTDTTT/BTL/code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ptiteduvn-my.sharepoint.com/personal/huytq_b20cn327_stu_ptit_edu_vn/Documents/Desktop/CHTDTTT/BTL/code/sinh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{C43CD6CE-B4BC-4CEA-83AD-67642F2934CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3664E9D-FA1B-4E6D-9AC0-6FDB5117D5FB}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{C43CD6CE-B4BC-4CEA-83AD-67642F2934CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07C6B750-AA5B-4FBA-B92A-CC0F981EA100}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{11A7FC23-E157-423F-8919-F627F9C29D18}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{11A7FC23-E157-423F-8919-F627F9C29D18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="280">
   <si>
     <t>S1</t>
   </si>
@@ -721,6 +723,159 @@
   </si>
   <si>
     <t>P8, SY54</t>
+  </si>
+  <si>
+    <t>M1, P1</t>
+  </si>
+  <si>
+    <t>M1, P2</t>
+  </si>
+  <si>
+    <t>M1, P3</t>
+  </si>
+  <si>
+    <t>M1, P4</t>
+  </si>
+  <si>
+    <t>M1, P5</t>
+  </si>
+  <si>
+    <t>M1, P6</t>
+  </si>
+  <si>
+    <t>M1, P7</t>
+  </si>
+  <si>
+    <t>M1, P8</t>
+  </si>
+  <si>
+    <t>ST1</t>
+  </si>
+  <si>
+    <t>ST2</t>
+  </si>
+  <si>
+    <t>ST3</t>
+  </si>
+  <si>
+    <t>ST4</t>
+  </si>
+  <si>
+    <t>ST5</t>
+  </si>
+  <si>
+    <t>Về vấn đề dinh dưỡng:\nCon bạn đang trong giai đoạn 1 - 2 tháng, trẻ bú mỗi 2 đến 3 tiếng suốt cả ngày lẫn đêm. Nếu con bạn bú ít hơn 480 ml sữa mỗi ngày cần bổ sung thêm vitamin D.\nVề vấn đề vận động\nBạn hãy khám phá đôi chân của trẻ bằng cách giữ chúng và nhẹ nhàng uốn cong, giúp kích thích cảm giác chạm và phát triển cơ bắp.</t>
+  </si>
+  <si>
+    <t>Về vấn đề dinh dưỡng:\nCon bạn đang trong giai đoạn 2 - 4 tháng, trẻ bú mỗi 3 đến 4 tiếng trong ngày. Nếu trẻ uống ít hơn 500ml sữa mỗi ngày có thể cần bổ sung thêm vitamin D.\nVề vấn đề vận động:\n Bố trí đồ chơi mà trẻ có thể nắm bằng tay, hỗ trợ phát triển cảm giác về tác động và khuyến khích sự chủ động từ bé.</t>
+  </si>
+  <si>
+    <t>Về vấn đề dinh dưỡng:\nCon bạn đang trong giai đoạn 4 - 6 tháng, trẻ bú mỗi 4 - 5 giờ mỗi ngày. Nếu trẻ uống ít hơn 480ml sữa công thức mỗi ngày đều cần được bổ sung thêm vitamin D. Về vấn đề vận động:\nBạn nên đặt trẻ nằm bụng để tăng cường cơ bắp vùng vai và cổ, đồng thời đặt đồ chơi ở xa để khuyến khích bé vươn tới và quay lăn để giúp bé phát triển cơ bắp.</t>
+  </si>
+  <si>
+    <t>Về vấn đề dinh dưỡng:\nCon bạn đang trong giai đoạn 6 - 7 tháng tuổi, trẻ nên được cho uống 720 – 960ml sữa mẹ hoặc sữa công thức một ngày chia làm 8 – 10 cữ, \nỞ giai đoạn này, trẻ có thể được cho ăn dặm. Bạn có thể tham khỏa thực đơn với nguyên liệu sau:\nBữa chính: ăn bột ngọt: bột gạo, bột lúa mì, bột từ củ: khoai tây, khoai lang, khoai mỡ pha với sữa để bé quen khẩu vị dần. \nBột loãng, chỉ đặc hơn sữa một chút\nMỗi ngày ăn 2 bữa vào khung thời gian cố định, mỗi bữa chỉ 2 – 3 muỗm cà phê từ từ tăng dần.\nTrong sữa mẹ đã cung cấp đủ nước cho trẻ nên trẻ không cần uống nước\nVề vấn đề vận động:\nBạn nên hỗ trợ bé khi đang cố gắng ngồi đứng, sử dụng ghế hỗ trợ hoặc gối để giữ thăng bằng và tăng cường sức mạnh cơ bắp.</t>
+  </si>
+  <si>
+    <t>Về vấn đề dinh dưỡng:\nCon bạn đang trong giai đoạn 7 – 9 tháng tuổi, trẻ nên được cho uống 720 – 960ml sữa mẹ hoặc sữa công thức mỗi ngày chia làm 8 – 10 cữ\nỞ giai đoạn này, trẻ đã được cho ăn dặm. Bạn có thể tham khảo thực đơn với nguyên liệu như sau:\nBữa chính: ăn các loại bột với thịt, rau say nhuyễn. Mỗi ngày 2 – 3 bữa vào khung thời gian cố định, mỗi bữa khoảng 100 – 120ml thức ăn, từ từ tăng dần\nBữa phụ: 1 – 2 bữa, gồm các loại trái cây mềm: chuối, xoài… Có thể mua các loại bánh ăn dặm dành riêng cho trẻ.\nCó thể cho trẻ tập uống nước sau mỗi bữa ăn dặm, mỗi lần 2 – 3 thìa cà phê.\nVề vấn đề vận động:\nBạn nên chơi cùng bé khuyến khích bé nâng đầu và ngực lên khi nằm bụng, đồng thời cung cấp đồ chơi để kích thích sự chủ động và tò mò.</t>
+  </si>
+  <si>
+    <t>Về vấn đề dinh dưỡng:\nCon bạn đang trong giai đoạn 9 – 12 tháng tuổi, trẻ nên được cho uống rẻ uống 500 – 600 ml sữa mẹ hoặc sữa công thức mỗi ngày, chia làm 4 – 5 cữ.\nỞ giai đoạn này, trẻ đã ăn dặm được một thời gian, tiếp tục khuyến khích trẻ ăn với thực đơn bạn có thể tham khảo như sau:\nBữa chính: trẻ có thể ăn cháo, với đầy đủ 4 nhóm: thịt(90 – 100g/ngày), bột/cháo, rau củ, dầu: 6 – 10ml. Chia làm 3 bữa, mỗi bữa 150 – 200ml thức ăn.\nBữa phụ: 1 – 2 bữa, gồm các loại trái cây mềm: chuối, xoài… Có thể mua các loại bánh ăn dặm dành riêng cho trẻ.\nVề vấn đề vận động:\n Đây là thời điểm quan trọng cho sự vận động của trẻ. Bạn nên cho bé cơ hội tự đứng và bám vào các đối tượng xung quanh, giúp phát triển sức mạnh và sự ổn định.</t>
+  </si>
+  <si>
+    <t>Về vấn đề dinh dưỡng:\nCon bạn đang trong giai đoạn trên 12 tháng tuổi\nNhững trẻ đang bú mẹ nên tiếp tục được cho bú. Bé từ 12 tháng tuổi có thể dừng uống sữa bột và chuyển sang uống sữa tươi nguyên kem. Một ngày bé nên uống 2 - 3 ly (0.47 lít tới 0.70 lít).\nNên tập cho trẻ uống tất cả các loại sữa nước hoa quả/thức ăn… bằng ly (cốc) thay vì bằng bình sữa để chống sâu răng. Hạn chế uống các loại nước hoa quả chứa vitamin C quá nhiều, không nên vượt quá 0.11 lít - 0.17 lít/ ngày, và khuyến khích bé uống nước lọc.\nDùng thực đơn cân bằng cho bé và khuyến khích bé ăn rau quả. Cho bé ăn 3 bữa chính và 2-3 bữa phụ trong một ngày. Cắt đồ ăn thành miếng nhỏ để bé không bị nghẹn.\nĐảm bảo cho bé tránh thức ăn có hàm luợng mỡ„ muối„ và đuờng cao. Dần dần giúp bé chuyển thực đơn sang bữa ăn bình thường của gia đình thay vì thức ăn đặc biệt cho trẻ nhỏ.\nCho bé ngồi ở ghế ăn cao ngang bàn để tăng giao tiếp của bé trong bữa ăn. Đừng ép bé ăn hết các đồ ăn trong đĩa.\nTránh cho bé ăn các loại hạt cứng„ kẹo cứng„ ngô bung„ và kẹo cao su để tránh bị dị vật đường thở do hít sặc khi nuốt.\nKhuyến khích bé tự ăn bằng thìa và có chén (bát) đĩa riêng.\nBé cần đánh răng sau bữa ăn và trước khi đi ngủ. Nếu dùng kem đánh răng cho trẻ thì nên dùng loại không chứa flo (Fluoride). Trong một số trường hợp bác sĩ có thể khuyên bổ sung flo (Fluoride) cho trẻ.\n Về vấn đề vận động:\nBạn nên khuyến khích bé đi bằng cách sử dụng đồ chơi hoặc đưa tay để hỗ trợ, đồng thời tạo các trò chơi vận động như chạy nhảy để phát triển sự linh hoạt và cân bằng.</t>
+  </si>
+  <si>
+    <t>Con bạn cần được bổ sung thêm sắt 2mg/kg mỗi ngày, tối đa 15mg/ngày/. Lượng sắt này được cung cấp đủ trong sữa công thức. Nếu trẻ bú sữa mẹ hoàn toàn, bạn có thể cho trẻ uống thuốc sắt dạng lỏng, siro cho đến khi trẻ có thể ăn dặm.</t>
+  </si>
+  <si>
+    <t>Trẻ từ 6 tháng tuổi trở đi nên bắt đầu cho trẻ ăn dặm bên cạnh uống sữa mẹ, nên bắt đầu với những thực phẩm giàu sắt. Bạn có thể xem xét bổ sung sắt dạng thực phẩm chức năng như thuốc lỏng 11mg mỗi ngày. Bổ sung sắt dạng này chủ yếu được dùng khi con bạn không thể ăn dặm với thức ăn đặc. Một số loại thực phẩm giàu sắt cho trẻ ăn dặm: các loại thịt: thịt bò, thịt lợn, thì gà,... Các lại hải sản: tôm, cua, cá hồi,... Các loại rau củ có màu đỏ, rau xanh như rau chân vịt, bông cải...Tăng cường các loại thực phẩm giàu vitamin C (như cam quýt, dâu tây, đu đủ, bông cải xanh…) sẽ góp phần giúp trẻ tăng hấp thu sắt.</t>
+  </si>
+  <si>
+    <t>Kinh nghiệm dành cho thai phụ: Phụ nữ có thai nên sử dụng viên sắt mỗi ngày, uống kéo dài tới sau khi sinh một tháng. Liều bổ sung là 60mg sắt mỗi ngày. Ngoài ra cũng nên sử dụng các thực phẩm có tăng cường sắt cho phụ nữ mang thai.</t>
+  </si>
+  <si>
+    <t>Con bạn từ 1 tuổi trở lên không nên uống quá nhiều sữa bò (quá 600ml sữa mỗi ngày), vì đây không phải là nguồn cung cấp sắt cho cơ thể. Hơn nữa, sữa bò có thể ức chế sự hấp thu sắt từ thức ăn khác.\nMột số loại thực phẩm giàu sắt cho trẻ ăn dặm: các loại thịt: thịt bò, thịt lợn, thì gà,... Các lại hải sản: tôm, cua, cá hồi,... Các loại rau củ có màu đỏ, rau xanh như rau chân vịt, bông cải...Tăng cường các loại thực phẩm giàu vitamin C (như cam quýt, dâu tây, đu đủ, bông cải xanh…) sẽ góp phần giúp trẻ tăng hấp thu sắt.</t>
+  </si>
+  <si>
+    <t>Con bạn dưới 6 tháng tuổi cần bổ sung 3mg kẽm mỗi ngày</t>
+  </si>
+  <si>
+    <t>Con bạn trong giai đoạn từ 6 – 12 tháng tuổi, trẻ cần được bổ sung 5 – 8 mg/ngày</t>
+  </si>
+  <si>
+    <t>Con bạn đang trong giai đoạn từ 1 tuổi – 2 tuổi cần khoảng 10 – 15 mg/ngày để phát triển chiều cao và thể chất tối ưu nhất.</t>
+  </si>
+  <si>
+    <t>Con bạn đang trong giai đoạn dưới 6 tháng tuổi nên nguồn kẽm tốt nhất và dễ hấp thu nhất đó chính là sữa mẹ. Lúc này hàm lượng kẽm trong sữa mẹ là 2-3mg/ lít, đáp ứng đủ tiêu chuẩn sử dụng. Do đó, bạn chỉ cần cho bé bú hoàn toàn trong 6 tháng đầu.</t>
+  </si>
+  <si>
+    <t>Con bạn đang trong gian đoạn trên 6 tháng tuổi, lượng kẽm trong sữa mẹ giảm dần, cần bổ sung kẽm qua thực phẩm ăn dặm cho trẻ. Một số thực phẩm giàu kẽm có thể bổ sung cho trẻ như tôm đồng, lươn, hàu, sò, gan lợn, sữa, thịt bò, lòng đỏ trứng, cá, đậu nành, các hạt có dầu (hạnh nhân, hạt điều, đậu phộng...). Để trẻ hấp thụ kẽm tốt nhất, bạn nên bổ sung vitamin C cho trẻ từ chính các loại trái cây tươi giàu lượng vitamin C sẵn có như cam, chanh, quýt, bưởi…</t>
+  </si>
+  <si>
+    <t>Kinh nghiệm dành cho thai phụ: phụ nữ mang thai cần bổ sung kẽm vào khẩu phần ăn hàng ngày để cung cấp cho thai nhi. Các nhóm thực phẩm giàu kẽm như tôm, cua, thịt, trứng, cá.</t>
+  </si>
+  <si>
+    <t>Nuôi con bằng sữa mẹ cũng là một trong những phương pháp nhằm phòng chống thiếu hụt vitamin D ở trẻ, bạn nên cho trẻ tắm nắng hàng ngày, mỗi ngày 20 – 30 phút vào buổi sáng là tốt nhất (trước 9 giờ), trường hợp không có điều kiện để tắm nắng như sinh vào mùa đông hoặc nhà ở chật chội... thì phải cho trẻ bổ sung vitamin D từ khi sinh ra sau 1 tuần, thời gian uống đến 2 tuổi, còn khi trẻ đã lớn, chơi được ngoài trời nhiều hơn hoặc không có biểu hiện của bệnh còi xương thì cũng không cần phải uống nữa.</t>
+  </si>
+  <si>
+    <t>Bạn cần bổ sung vitamin D vào khẩu phần ăn của trẻ như sữa, phomat, bánh quy, dầu ăn, các loại ngũ cốc hay bột dinh dưỡng.. Trong rau xanh có vitamin D là yếu tố hình thành osteocalcin, osteocalcin giúp tích tụ canxi vào xương.Vitamin D và canxi là bộ đôi “ăn ý” không thể tách rời bởi vì vitamin D là chất dẫn truyền giúp cho cơ thể bé hấp thu canxi tốt hơn. Có thể bổ sung vitamin D qua các loại thực phẩm giàu loại vitamin này như sữa, sữa chua, lòng đỏ trứng, cá hồi, dầu gan cá,…</t>
+  </si>
+  <si>
+    <t>Kinh nghiệm dành cho thai phụ: phụ nữa có thai và cho con bú cần ăn nhiều thức ăn giàu vitamin A, ăn tăng dầu mỡ. Cho trẻ bú sớm, ngay sau đẻ từ 30 phút đến 1 giờ, bú hoàn toàn trong 4 - 6 tháng đầu, bú kéo dài 18 - 24 tháng.</t>
+  </si>
+  <si>
+    <t>Con bạn cần được uống bổ sung vitamin A định kỳ hằng năm, mỗi năm 2 lần. Con bạn dưới 6 tháng tuổi, cần bổ sung 50.000 đơn vị vitamin A.</t>
+  </si>
+  <si>
+    <t>Con bạn cần được uống bổ sung vitamin A định kỳ hằng năm, mỗi năm 2 lần. Con bạn đang trong giai đoạn từ 6-12 tháng tuổi, cần bổ sung 100.000 đơn vị vitamin A. Một số thực phẩm giàu vitamin A thích hợp cho trẻ : bí ngô, cà rốt, khoai lang, gan, trứng, dầu cá hồi, quả mâm xôi,... Bạn có thể cắt nhỏ hoặc nghiền thêm vào bữa ăn dặm cho trẻ, vừa tăng màu sắc và hương vị giúp trẻ ngon miệng vừa bổ sung chất dinh dưỡng tốt cho sự phát triển của trẻ.</t>
+  </si>
+  <si>
+    <t>Con bạn cần được uống bổ sung vitamin A định kỳ hằng năm, mỗi năm 2 lần. Con bạn đang trong giai đoạn từ 12 - 24 tháng tuổi, cần bổ sung 200.000 đơn vị vitamin A. Một số thực phẩm giàu vitamin A thích hợp cho trẻ : bí ngô, cà rốt, khoai lang, gan, trứng, dầu cá hồi, quả mâm xôi,... Bạn có thể cắt nhỏ hoặc nghiền thêm vào bữa ăn dặm cho trẻ, vừa tăng màu sắc và hương vị giúp trẻ ngon miệng vừa bổ sung chất dinh dưỡng tốt cho sự phát triển của trẻ.</t>
+  </si>
+  <si>
+    <t>Bạn nên xây dựng chế độ ăn uống cân bằng, đa dạng, bổ sung vào thực đơn ăn dặm cho trẻ, bao gồm nhiều loại thực phẩm giàu chất béo. Cách bổ sung tốt nhất để đảm bảo lưu giữ trọn vẹn dưỡng chất có lợi là trộn dầu dinh dưỡng đặc chế cho trẻ vào thức ăn còn nóng (cháo, bột, cơm khi vừa nấu xong) với liều lượng 10ml/ngày (nếu trẻ ăn 2 bữa chính/ngày thì mỗi bữa trộn 1 muỗng café – 5ml).\nNhằm đảm bảo cung cấp đúng và đủ các chất béo cần biết, bạn cần cho trẻ ăn đa dạng thực phẩm như các loại mỡ (mỡ bò, lợn và cừu), thịt, trứng, sữa, đặc biệt là các loại cá béo (cá hồi, cá ngừ, cá trích…) do đây là nguồn cung cấp Omega 3 (EPA và DHA) dồi dào.\nMột số thực phẩm giàu chất béo bao gồm:\nThực phẩm giàu chất béo lành mạnh:\nDầu ô liu\nDầu hạt cải\nDầu hạt hướng dương\nDầu đậu nành\nHạt chia\nHạt lanh\nCác loại hạt: hạnh nhân, hạt óc chó, quả hồ trăn\nCác loại đậu: đậu nành, đậu đen, đậu Hà Lan\nThực phẩm giàu chất béo bão hòa:\nThịt đỏ\nSữa và các sản phẩm từ sữa\nTrứng</t>
+  </si>
+  <si>
+    <t>Con của bạn đang trong giai đoạn dưới 6 tháng tuổi nên được bú mẹ hoàn toàn nhằm nâng cao sức đề kháng và hệ miễn dịch. Điều này không chỉ giúp giảm nguy cơ béo phì ở trẻ mà còn giúp trẻ tránh được một số bệnh lý khác.</t>
+  </si>
+  <si>
+    <t>Con bạn trong giai đoạn từ 0 - 6 tháng tuổi, nhu cầu iốt của trẻ là 40mcg/ngày. Trẻ bú mẹ hoàn toàn, do đó bạn nên ăn nhiều hải sản và dùng muối i ốt hoặc nước mắm có iốt để nguồn dưỡng chất quan trọng này tiết qua sữa bổ sung cho bé.</t>
+  </si>
+  <si>
+    <t>Con bạn trong giai đoạn từ 6 tháng tuổi, nhu cầu Iot của trẻ là 50mcg/ngày. Trẻ đã có thể ăn dặm nên bạn cần bổ sung iốt qua ăn uống hàng ngày. Iốt có nhiều trong hải sản: cá, tôm, cua và có nhiều trong các loại rau như rong, tảo biển, rau câu, rau xanh...\nTrứng và các thực phẩm từ sữa cũng là một nguồn cung cấp iốt khá tốt. Vì vậy, bạn chú ý thêm vào thực đơn cho bé từ nguồn thức ăn giàu iốt này.</t>
+  </si>
+  <si>
+    <t>Ở mỗi độ tuổi trẻ sẽ có nhu cầu canxi khác nhau, cụ thể: con bạn dưới 6 tháng tuổi sẽ cần 300mg canxi/ ngày.\n Bạn cũng cần chú ý đến việc tăng cường canxi cho bản thân để cung cấp đủ canxi trong sữa cho trẻ. Các thực phẩm giàu canxi nhu sữa, trứng. Các loại hạt, ngũ cốc: hạt mè, hạt điều, quả óc chó,...Các loại thuỷ hải sản: Tôm cua, sò... \n. Bạn và trẻ cần được hấp thụ vitamin D qua việc tắm nắng. Thời gian tắm nắng tốt nhất khoảng từ 7 - 9 giờ sáng hoặc 5 - 6 giờ chiều. Mỗi lần khoảng 15 - 20 phút</t>
+  </si>
+  <si>
+    <t>Ở mỗi độ tuổi trẻ sẽ có nhu cầu canxi khác nhau, cụ thể: con bạn trong giai đoạn 6 tháng tới 12 tháng tuổi cần 400mg canxi/ ngày.</t>
+  </si>
+  <si>
+    <t>Để bổ sung canxi cho bé qua đường ăn uống bạn có thể mua các loại thực phẩm như hải sản gồm cá, cua, tôm sò,… hay các loại rau cải xoăn, cần tây, bắp cải, diếp cá để tăng cường sức khỏe cho xương. Trong rau xanh có vitamin D là yếu tố hình thành osteocalcin, osteocalcin giúp tích tụ canxi vào xương.Kết hợp với vitamin DVitamin D và canxi là bộ đôi “ăn ý” không thể tách rời bởi vì vitamin D là chất dẫn truyền giúp cho cơ thể bé hấp thu canxi tốt hơn. Do vậy để trẻ hấp thu tốt nhất lượng canxi vào cơ thể bạn nên bổ sung cả vitamin D cho trẻ. Có thể bổ sung vitamin D bằng cách cho trẻ phơi nắng vào buổi sáng sớm hoặc qua các loại thực phẩm giàu loại vitamin này như sữa, sữa chua, lòng đỏ trứng, cá hồi, dầu gan cá,…</t>
+  </si>
+  <si>
+    <t>Trẻ có cân nặng dưới mức bình thường đối với độ tuổi và chiều cao của trẻ. Bạn cần cân bằng lại chế độ dinh dưỡng cho trẻ. Bổ sung thêm các nhóm thức ăn như rau củ, trái cây, ngũ cốc, thịt, cá, sữa và sản phẩm từ sữa. Bổ sung thêm bữa ăn nhẹ để cung cấp năng lượng và chất dinh dưỡng liên tục trong ngày.</t>
+  </si>
+  <si>
+    <t>Trẻ có cân nặng và chiều cao đều thấp so với tiêu chuẩn độ tuổi. Bạn cần bổ sung chế độ ăn giàu năng lượng cho trẻ. đặc biệt là từ chất béo và carbohydrate, để hỗ trợ tăng cân và phát triển. Bổ sung protein từ thực phẩm như thịt, cá, trứng và đậu nành để hỗ trợ xây dựng cơ bắp.</t>
+  </si>
+  <si>
+    <t>Trẻ có cơ thể gầy, thiếu mỡ, và có thể xuất hiện tình trạng suy nhược cơ bắp. Bạn cần tăng cường thêm nguồn protein từ thức ăn như thịt, cá, trứng, sữa, đậu nành, và thậm chí có thể xem xét sử dụng bổ sung protein nếu cần. Phân chia thức ăn thành nhiều bữa nhỏ trong ngày để cung cấp năng lượng và chất dinh dưỡng liên tục.</t>
+  </si>
+  <si>
+    <t>Ở mỗi độ tuổi trẻ sẽ có nhu cầu canxi khác nhau, cụ thể: con bạn trong giai đoạn từ 1 đến 2 tuổi cần 500 mg canxi/ngày.</t>
+  </si>
+  <si>
+    <t>Trẻ có chiều cao cân nặng bình thường, phù hợp với sự phát triển ở độ tuổi của mình. Để đảm bảo sự phát triển toàn diện, chế độ ăn cần được thiết kế đa dạng và cân đối, tập trung vào rau củ, trái cây, ngũ cốc nguyên hạt, thịt, cá, và sản phẩm từ sữa. Các thức ăn nên được chế biến nhẹ nhàng để bảo toàn chất dinh dưỡng và hạn chế đường cũng như muối. Cha mẹ nên khuyến khích trẻ tham gia vào các hoạt động vận động, như chơi ngoài trời và nhảy lò cò, để phát triển cơ bắp và kỹ năng cân bằng. Môi trường gia đình nên làm cho thời gian ăn trở thành một trải nghiệm tích cực và khuyến khích lối sống lành mạnh.</t>
+  </si>
+  <si>
+    <t>Trẻ có cân nặng vượt chuẩn và có dấu hiệu của thừa cân béo phì. Cha mẹ hãy xem xét lại và đảm bảo rằng chế độ ăn của trẻ là cân đối và giàu chất dinh dưỡng, hạn chế thức ăn nhanh và đồ ngọt. Khuyến khích trẻ tham gia hoạt động vận động hàng ngày như chơi ngoài trời hoặc các trò chơi tập luyện để giúp đốt cháy calo và tăng cường sức khỏe. Sử dụng các dụng cụ đo hoặc bát kích thước để kiểm soát lượng thức ăn. Gia đình có thể hỗ trợ bằng cách tham gia vào quá trình chuẩn bị và thưởng thức các bữa ăn lành mạnh cùng nhau. Đồng thời, giảm thời gian trẻ tiếp xúc với màn hình điện thoại hay máy tính bảng và khuyến khích hoạt động, chơi đùa. Đảm bảo trẻ có đủ giấc ngủ sẽ giúp kiểm soát hormone đói và no, hỗ trợ quá trình quản lý cân nặng.</t>
+  </si>
+  <si>
+    <t>Điều chỉnh chế độ dinh dưỡng:Bạn cần điều chỉnh chế độ dinh dưỡng của mình và cho bé theo hướng lành mạnh. Đảm bảo cung cấp đủ nhóm chất, ưu tiên rau xanh và hoa quả, đạm, hạn chếchất béo và tinh bột không tốt, dầu mỡ. Nếu bé dùng sữa công thức, hãy ưu tiên sữa tăng cân vừa phải và chọn sữa phù hợp cho giai đoạn phát triển của bé. Tăng cường vận động: Khuyến khích bé vận động bằng cách chơi trò chơi cùng bé, thực hiện các động tác nhẹ nhàng hoặc hỗ trợ bé tập các kỹ năng mới. Điều này giúp bé tiến bộ nhanh hơn và giảm nguy cơ béo phì.Theo dõi cân nặng và sức khỏe: Ba mẹ nên theo dõi cân nặng của bé thường xuyên nếu bé có nguy cơ hoặc đã bị béo phì. Đồng thời, điều chỉnh chế độ dinh dưỡng, tăng cường vận động và sinh hoạt phù hợp để giúp bé tăng trưởng tốt.</t>
+  </si>
+  <si>
+    <t>Về vấn đề dinh dưỡng:\nCon bạn đang trong giai đoạn 0 - 1 tháng, nên trẻ có thể bú sữa công thức có bổ sung chất sắt nếu trẻ không thể bú mẹ hoàn toàn.\n Cứ 2 đến 3 tiếng thì nên cho trẻ bú một lần. Bạn cho trẻ bú ít hơn 473 ml sữa một ngày và cần được bổ sung thêm vitamin D.\nVề vấn đề vận động, trong giai đoạn này, đặt trẻ nằm ngD2:D29ửa và khích lệ chúng nhìn về các đối tượng sáng và đơn giản để phát triển khả năng quan sát của bé.</t>
   </si>
 </sst>
 </file>
@@ -748,7 +903,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -758,6 +913,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -850,7 +1011,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -881,6 +1042,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1199,8 +1366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D492B16-5BBC-4C99-BB10-F54B80A61577}">
   <dimension ref="C1:F398"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A378" workbookViewId="0">
-      <selection activeCell="E253" sqref="E253:F398"/>
+    <sheetView topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="E295" sqref="E295:F398"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6775,4 +6942,916 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6333E0C-839D-4266-94F2-21F46EC8931A}">
+  <dimension ref="C1:D86"/>
+  <sheetViews>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D86"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="46.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="D7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D30" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D33" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D34" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D37" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D38" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D39" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>164</v>
+      </c>
+      <c r="D40" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>165</v>
+      </c>
+      <c r="D42" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D43" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>167</v>
+      </c>
+      <c r="D44" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>168</v>
+      </c>
+      <c r="D45" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>169</v>
+      </c>
+      <c r="D46" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>170</v>
+      </c>
+      <c r="D47" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>171</v>
+      </c>
+      <c r="D48" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>193</v>
+      </c>
+      <c r="D50" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>194</v>
+      </c>
+      <c r="D51" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>195</v>
+      </c>
+      <c r="D52" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>196</v>
+      </c>
+      <c r="D53" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>197</v>
+      </c>
+      <c r="D54" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>198</v>
+      </c>
+      <c r="D55" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>199</v>
+      </c>
+      <c r="D56" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>200</v>
+      </c>
+      <c r="D57" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>201</v>
+      </c>
+      <c r="D58" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>202</v>
+      </c>
+      <c r="D59" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>203</v>
+      </c>
+      <c r="D60" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>204</v>
+      </c>
+      <c r="D61" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>205</v>
+      </c>
+      <c r="D62" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>206</v>
+      </c>
+      <c r="D63" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>207</v>
+      </c>
+      <c r="D64" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>208</v>
+      </c>
+      <c r="D65" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>209</v>
+      </c>
+      <c r="D66" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>210</v>
+      </c>
+      <c r="D67" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>211</v>
+      </c>
+      <c r="D68" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>212</v>
+      </c>
+      <c r="D69" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>213</v>
+      </c>
+      <c r="D70" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>214</v>
+      </c>
+      <c r="D71" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>215</v>
+      </c>
+      <c r="D72" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>216</v>
+      </c>
+      <c r="D73" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>186</v>
+      </c>
+      <c r="D74" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>187</v>
+      </c>
+      <c r="D75" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>188</v>
+      </c>
+      <c r="D76" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>85</v>
+      </c>
+      <c r="D77" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>186</v>
+      </c>
+      <c r="D78" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>187</v>
+      </c>
+      <c r="D79" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>188</v>
+      </c>
+      <c r="D80" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>85</v>
+      </c>
+      <c r="D81" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>237</v>
+      </c>
+      <c r="D82" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>238</v>
+      </c>
+      <c r="D83" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>239</v>
+      </c>
+      <c r="D84" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>240</v>
+      </c>
+      <c r="D85" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>241</v>
+      </c>
+      <c r="D86" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9588B68-3678-41F6-884A-31019138DF57}">
+  <dimension ref="D1:D39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D39" sqref="D2:D39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="160.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="4:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="3" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="4:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="12" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="7" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="8" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="12" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="9" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="12" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="10" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="13" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="12" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="14" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="15" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="13" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="16" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="13" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="12" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="12" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="12" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="12" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="12" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="3" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D34" s="12" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="12" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D39" s="12" t="s">
+        <v>277</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>